<commit_message>
updates to DY run files using standard_pipeline
stepping back from full pipeline temporarily
</commit_message>
<xml_diff>
--- a/runs/DY/manifest.xlsx
+++ b/runs/DY/manifest.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11200" yWindow="1880" windowWidth="36320" windowHeight="23280"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="33600" windowHeight="20460"/>
   </bookViews>
   <sheets>
     <sheet name="SampleInfo" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="223">
   <si>
     <t>OldName</t>
   </si>
@@ -656,6 +656,42 @@
   </si>
   <si>
     <t>PanCancer Panel V1.2</t>
+  </si>
+  <si>
+    <t>Pan_Cancer_F1_IGO_05500_DY_42</t>
+  </si>
+  <si>
+    <t>Pan_Cancer_F10_IGO_05500_DY_38</t>
+  </si>
+  <si>
+    <t>Pan_Cancer_F3_IGO_05500_DY_36</t>
+  </si>
+  <si>
+    <t>Pan_Cancer_F4_IGO_05500_DY_43</t>
+  </si>
+  <si>
+    <t>Pan_Cancer_F6_IGO_05500_DY_37</t>
+  </si>
+  <si>
+    <t>Pan_Cancer_F8_IGO_05500_DY_44</t>
+  </si>
+  <si>
+    <t>Pan_Cancer_M1_IGO_05500_DY_45</t>
+  </si>
+  <si>
+    <t>Pan_Cancer_M2_IGO_05500_DY_39</t>
+  </si>
+  <si>
+    <t>Pan_Cancer_M6_IGO_05500_DY_46</t>
+  </si>
+  <si>
+    <t>Pan_Cancer_M7_IGO_05500_DY_40</t>
+  </si>
+  <si>
+    <t>Pan_Cancer_M8_IGO_05500_DY_47</t>
+  </si>
+  <si>
+    <t>Pan_Cancer_M9_IGO_05500_DY_41</t>
   </si>
 </sst>
 </file>
@@ -1307,7 +1343,7 @@
   <dimension ref="A1:W48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2677,7 +2713,7 @@
     </row>
     <row r="20" spans="1:23">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>211</v>
       </c>
       <c r="B20" t="s">
         <v>49</v>
@@ -2748,7 +2784,7 @@
     </row>
     <row r="21" spans="1:23">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>212</v>
       </c>
       <c r="B21" t="s">
         <v>63</v>
@@ -2819,7 +2855,7 @@
     </row>
     <row r="22" spans="1:23" s="120" customFormat="1">
       <c r="A22" s="120" t="s">
-        <v>4</v>
+        <v>213</v>
       </c>
       <c r="B22" s="120" t="s">
         <v>5</v>
@@ -2890,7 +2926,7 @@
     </row>
     <row r="23" spans="1:23">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>214</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
@@ -2961,7 +2997,7 @@
     </row>
     <row r="24" spans="1:23">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>215</v>
       </c>
       <c r="B24" t="s">
         <v>87</v>
@@ -3032,7 +3068,7 @@
     </row>
     <row r="25" spans="1:23">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>216</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
@@ -3103,7 +3139,7 @@
     </row>
     <row r="26" spans="1:23">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>217</v>
       </c>
       <c r="B26" t="s">
         <v>47</v>
@@ -3174,7 +3210,7 @@
     </row>
     <row r="27" spans="1:23">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>218</v>
       </c>
       <c r="B27" t="s">
         <v>67</v>
@@ -3245,7 +3281,7 @@
     </row>
     <row r="28" spans="1:23">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>219</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -3316,7 +3352,7 @@
     </row>
     <row r="29" spans="1:23">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>220</v>
       </c>
       <c r="B29" t="s">
         <v>89</v>
@@ -3387,7 +3423,7 @@
     </row>
     <row r="30" spans="1:23">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>221</v>
       </c>
       <c r="B30" t="s">
         <v>81</v>
@@ -3458,7 +3494,7 @@
     </row>
     <row r="31" spans="1:23">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>222</v>
       </c>
       <c r="B31" t="s">
         <v>95</v>

</xml_diff>